<commit_message>
update Yihan's task status
</commit_message>
<xml_diff>
--- a/PRD/Concrete timeline_15.06.18.xlsx
+++ b/PRD/Concrete timeline_15.06.18.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="27700" windowHeight="16480" tabRatio="500"/>
+    <workbookView xWindow="1600" yWindow="1340" windowWidth="26880" windowHeight="15580" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="62">
   <si>
     <t>Stella</t>
   </si>
@@ -579,6 +579,54 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="17" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="17" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="17" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="17" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="17" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -599,54 +647,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="17" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="17" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="17" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="17" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -930,8 +930,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R197"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="75" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="75" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="Q9" sqref="Q9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -946,7 +946,7 @@
     <col min="8" max="9" width="16.6640625" style="6" customWidth="1"/>
     <col min="10" max="10" width="10.83203125" style="6" customWidth="1"/>
     <col min="11" max="11" width="18.83203125" style="6" customWidth="1"/>
-    <col min="12" max="12" width="29.33203125" style="59" customWidth="1"/>
+    <col min="12" max="12" width="35.83203125" style="59" customWidth="1"/>
     <col min="13" max="13" width="10" style="6" customWidth="1"/>
     <col min="14" max="14" width="18.6640625" style="41" customWidth="1"/>
     <col min="15" max="15" width="11.5" style="7" customWidth="1"/>
@@ -956,22 +956,22 @@
   <sheetData>
     <row r="1" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2"/>
-      <c r="B1" s="81" t="s">
+      <c r="B1" s="72" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="81"/>
-      <c r="D1" s="81"/>
-      <c r="E1" s="81"/>
-      <c r="F1" s="81"/>
-      <c r="G1" s="82"/>
-      <c r="H1" s="79" t="s">
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
+      <c r="E1" s="72"/>
+      <c r="F1" s="72"/>
+      <c r="G1" s="73"/>
+      <c r="H1" s="70" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="80"/>
-      <c r="J1" s="80"/>
-      <c r="K1" s="80"/>
-      <c r="L1" s="80"/>
-      <c r="M1" s="80"/>
+      <c r="I1" s="71"/>
+      <c r="J1" s="71"/>
+      <c r="K1" s="71"/>
+      <c r="L1" s="71"/>
+      <c r="M1" s="71"/>
       <c r="N1" s="38" t="s">
         <v>10</v>
       </c>
@@ -983,51 +983,51 @@
     </row>
     <row r="2" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
-      <c r="B2" s="83" t="s">
+      <c r="B2" s="74" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="84"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
-      <c r="F2" s="84"/>
-      <c r="G2" s="84"/>
-      <c r="H2" s="84"/>
-      <c r="I2" s="84"/>
-      <c r="J2" s="84"/>
-      <c r="K2" s="84"/>
-      <c r="L2" s="84"/>
-      <c r="M2" s="84"/>
-      <c r="N2" s="84"/>
-      <c r="O2" s="84"/>
-      <c r="P2" s="84"/>
-      <c r="Q2" s="85"/>
+      <c r="C2" s="75"/>
+      <c r="D2" s="75"/>
+      <c r="E2" s="75"/>
+      <c r="F2" s="75"/>
+      <c r="G2" s="75"/>
+      <c r="H2" s="75"/>
+      <c r="I2" s="75"/>
+      <c r="J2" s="75"/>
+      <c r="K2" s="75"/>
+      <c r="L2" s="75"/>
+      <c r="M2" s="75"/>
+      <c r="N2" s="75"/>
+      <c r="O2" s="75"/>
+      <c r="P2" s="75"/>
+      <c r="Q2" s="76"/>
     </row>
     <row r="3" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="71" t="s">
+      <c r="B3" s="87" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="72"/>
+      <c r="C3" s="88"/>
       <c r="D3" s="62" t="s">
         <v>38</v>
       </c>
-      <c r="E3" s="73" t="s">
+      <c r="E3" s="89" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="72"/>
+      <c r="F3" s="88"/>
       <c r="G3" s="63" t="s">
         <v>38</v>
       </c>
-      <c r="H3" s="88" t="s">
+      <c r="H3" s="79" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="88"/>
+      <c r="I3" s="79"/>
       <c r="J3" s="52" t="s">
         <v>38</v>
       </c>
-      <c r="K3" s="74" t="s">
+      <c r="K3" s="90" t="s">
         <v>3</v>
       </c>
-      <c r="L3" s="75"/>
+      <c r="L3" s="91"/>
       <c r="M3" s="9" t="s">
         <v>38</v>
       </c>
@@ -1186,11 +1186,15 @@
       <c r="N6" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="O6" s="50"/>
+      <c r="O6" s="50" t="s">
+        <v>40</v>
+      </c>
       <c r="P6" s="44" t="s">
         <v>25</v>
       </c>
-      <c r="Q6" s="51"/>
+      <c r="Q6" s="51" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="7" spans="1:18" ht="240" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
@@ -1272,7 +1276,9 @@
       <c r="P8" s="44" t="s">
         <v>25</v>
       </c>
-      <c r="Q8" s="51"/>
+      <c r="Q8" s="51" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="9" spans="1:18" ht="144" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
@@ -1313,31 +1319,33 @@
       <c r="P9" s="44" t="s">
         <v>25</v>
       </c>
-      <c r="Q9" s="51"/>
+      <c r="Q9" s="51" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="10" spans="1:18" ht="32" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>46174</v>
       </c>
-      <c r="B10" s="77" t="s">
+      <c r="B10" s="82" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="78"/>
+      <c r="C10" s="80"/>
       <c r="D10" s="65"/>
-      <c r="E10" s="78" t="s">
+      <c r="E10" s="80" t="s">
         <v>23</v>
       </c>
-      <c r="F10" s="89"/>
+      <c r="F10" s="81"/>
       <c r="G10" s="68"/>
-      <c r="H10" s="90" t="s">
+      <c r="H10" s="83" t="s">
         <v>23</v>
       </c>
-      <c r="I10" s="91"/>
+      <c r="I10" s="84"/>
       <c r="J10" s="56"/>
-      <c r="K10" s="91" t="s">
+      <c r="K10" s="84" t="s">
         <v>23</v>
       </c>
-      <c r="L10" s="92"/>
+      <c r="L10" s="85"/>
       <c r="M10" s="57"/>
       <c r="N10" s="42" t="s">
         <v>27</v>
@@ -1352,25 +1360,25 @@
       <c r="A11" s="3">
         <v>46539</v>
       </c>
-      <c r="B11" s="77" t="s">
+      <c r="B11" s="82" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="78"/>
+      <c r="C11" s="80"/>
       <c r="D11" s="65"/>
-      <c r="E11" s="78" t="s">
+      <c r="E11" s="80" t="s">
         <v>29</v>
       </c>
-      <c r="F11" s="89"/>
+      <c r="F11" s="81"/>
       <c r="G11" s="68"/>
-      <c r="H11" s="90" t="s">
+      <c r="H11" s="83" t="s">
         <v>29</v>
       </c>
-      <c r="I11" s="91"/>
+      <c r="I11" s="84"/>
       <c r="J11" s="56"/>
-      <c r="K11" s="91" t="s">
+      <c r="K11" s="84" t="s">
         <v>29</v>
       </c>
-      <c r="L11" s="92"/>
+      <c r="L11" s="85"/>
       <c r="M11" s="57"/>
       <c r="N11" s="42" t="s">
         <v>28</v>
@@ -1382,45 +1390,45 @@
       <c r="Q11" s="51"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B12" s="86" t="s">
+      <c r="B12" s="77" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="87"/>
-      <c r="D12" s="87"/>
-      <c r="E12" s="87"/>
-      <c r="F12" s="87"/>
-      <c r="G12" s="87"/>
-      <c r="H12" s="87"/>
-      <c r="I12" s="87"/>
-      <c r="J12" s="87"/>
-      <c r="K12" s="87"/>
-      <c r="L12" s="87"/>
-      <c r="M12" s="87"/>
-      <c r="N12" s="87"/>
-      <c r="O12" s="87"/>
-      <c r="P12" s="87"/>
-      <c r="Q12" s="87"/>
+      <c r="C12" s="78"/>
+      <c r="D12" s="78"/>
+      <c r="E12" s="78"/>
+      <c r="F12" s="78"/>
+      <c r="G12" s="78"/>
+      <c r="H12" s="78"/>
+      <c r="I12" s="78"/>
+      <c r="J12" s="78"/>
+      <c r="K12" s="78"/>
+      <c r="L12" s="78"/>
+      <c r="M12" s="78"/>
+      <c r="N12" s="78"/>
+      <c r="O12" s="78"/>
+      <c r="P12" s="78"/>
+      <c r="Q12" s="78"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B13" s="71" t="s">
+      <c r="B13" s="87" t="s">
         <v>2</v>
       </c>
-      <c r="C13" s="72"/>
+      <c r="C13" s="88"/>
       <c r="D13" s="63"/>
-      <c r="E13" s="73" t="s">
+      <c r="E13" s="89" t="s">
         <v>3</v>
       </c>
-      <c r="F13" s="72"/>
+      <c r="F13" s="88"/>
       <c r="G13" s="63"/>
-      <c r="H13" s="76" t="s">
+      <c r="H13" s="92" t="s">
         <v>2</v>
       </c>
-      <c r="I13" s="74"/>
-      <c r="J13" s="75"/>
-      <c r="K13" s="74" t="s">
+      <c r="I13" s="90"/>
+      <c r="J13" s="91"/>
+      <c r="K13" s="90" t="s">
         <v>3</v>
       </c>
-      <c r="L13" s="74"/>
+      <c r="L13" s="90"/>
       <c r="M13" s="10"/>
       <c r="N13" s="39" t="s">
         <v>39</v>
@@ -1547,9 +1555,9 @@
       <c r="F17" s="28"/>
       <c r="G17" s="66"/>
       <c r="L17" s="40"/>
-      <c r="N17" s="70"/>
-      <c r="O17" s="70"/>
-      <c r="P17" s="70"/>
+      <c r="N17" s="86"/>
+      <c r="O17" s="86"/>
+      <c r="P17" s="86"/>
       <c r="Q17" s="31"/>
     </row>
     <row r="18" spans="1:17" s="24" customFormat="1" x14ac:dyDescent="0.2">
@@ -3174,6 +3182,15 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="N17:P17"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="H13:J13"/>
+    <mergeCell ref="K13:L13"/>
+    <mergeCell ref="B10:C10"/>
     <mergeCell ref="H1:M1"/>
     <mergeCell ref="B1:G1"/>
     <mergeCell ref="B2:Q2"/>
@@ -3186,15 +3203,6 @@
     <mergeCell ref="K10:L10"/>
     <mergeCell ref="H11:I11"/>
     <mergeCell ref="K11:L11"/>
-    <mergeCell ref="N17:P17"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="H13:J13"/>
-    <mergeCell ref="K13:L13"/>
-    <mergeCell ref="B10:C10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update critical feedback on Stella's code
</commit_message>
<xml_diff>
--- a/PRD/Concrete timeline_15.06.18.xlsx
+++ b/PRD/Concrete timeline_15.06.18.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="63">
   <si>
     <t>Stella</t>
   </si>
@@ -215,6 +215,11 @@
   </si>
   <si>
     <t>2. Do up data storage for set-up: study conditions etc. (KIV, model after Yihan's); Organize variables and scripts to correspond to conditions and studies</t>
+  </si>
+  <si>
+    <t>Critical feedback on previous day's work: 1. Please revise scale according to this example  https://wkwsci.co1.qualtrics.com/jfe/form/SV_eP3DmZu9T34ChqB
+2. Change visual advisor to “your personal financial advisor”
+3. Stage 0: both of Study and Conditions need to be highlighted</t>
   </si>
 </sst>
 </file>
@@ -579,6 +584,33 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="17" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -609,15 +641,9 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="17" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="17" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="17" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="17" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -626,27 +652,6 @@
     </xf>
     <xf numFmtId="17" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -931,7 +936,7 @@
   <dimension ref="A1:R197"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="75" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="Q9" sqref="Q9"/>
+      <selection activeCell="R7" sqref="R7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -956,22 +961,22 @@
   <sheetData>
     <row r="1" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2"/>
-      <c r="B1" s="72" t="s">
+      <c r="B1" s="81" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="72"/>
-      <c r="D1" s="72"/>
-      <c r="E1" s="72"/>
-      <c r="F1" s="72"/>
-      <c r="G1" s="73"/>
-      <c r="H1" s="70" t="s">
+      <c r="C1" s="81"/>
+      <c r="D1" s="81"/>
+      <c r="E1" s="81"/>
+      <c r="F1" s="81"/>
+      <c r="G1" s="82"/>
+      <c r="H1" s="79" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="71"/>
-      <c r="J1" s="71"/>
-      <c r="K1" s="71"/>
-      <c r="L1" s="71"/>
-      <c r="M1" s="71"/>
+      <c r="I1" s="80"/>
+      <c r="J1" s="80"/>
+      <c r="K1" s="80"/>
+      <c r="L1" s="80"/>
+      <c r="M1" s="80"/>
       <c r="N1" s="38" t="s">
         <v>10</v>
       </c>
@@ -983,51 +988,51 @@
     </row>
     <row r="2" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
-      <c r="B2" s="74" t="s">
+      <c r="B2" s="83" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="75"/>
-      <c r="D2" s="75"/>
-      <c r="E2" s="75"/>
-      <c r="F2" s="75"/>
-      <c r="G2" s="75"/>
-      <c r="H2" s="75"/>
-      <c r="I2" s="75"/>
-      <c r="J2" s="75"/>
-      <c r="K2" s="75"/>
-      <c r="L2" s="75"/>
-      <c r="M2" s="75"/>
-      <c r="N2" s="75"/>
-      <c r="O2" s="75"/>
-      <c r="P2" s="75"/>
-      <c r="Q2" s="76"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="84"/>
+      <c r="G2" s="84"/>
+      <c r="H2" s="84"/>
+      <c r="I2" s="84"/>
+      <c r="J2" s="84"/>
+      <c r="K2" s="84"/>
+      <c r="L2" s="84"/>
+      <c r="M2" s="84"/>
+      <c r="N2" s="84"/>
+      <c r="O2" s="84"/>
+      <c r="P2" s="84"/>
+      <c r="Q2" s="85"/>
     </row>
     <row r="3" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="87" t="s">
+      <c r="B3" s="71" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="88"/>
+      <c r="C3" s="72"/>
       <c r="D3" s="62" t="s">
         <v>38</v>
       </c>
-      <c r="E3" s="89" t="s">
+      <c r="E3" s="73" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="88"/>
+      <c r="F3" s="72"/>
       <c r="G3" s="63" t="s">
         <v>38</v>
       </c>
-      <c r="H3" s="79" t="s">
+      <c r="H3" s="88" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="79"/>
+      <c r="I3" s="88"/>
       <c r="J3" s="52" t="s">
         <v>38</v>
       </c>
-      <c r="K3" s="90" t="s">
+      <c r="K3" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="L3" s="91"/>
+      <c r="L3" s="75"/>
       <c r="M3" s="9" t="s">
         <v>38</v>
       </c>
@@ -1196,7 +1201,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="240" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18" ht="272" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>45078</v>
       </c>
@@ -1233,9 +1238,11 @@
       </c>
       <c r="O7" s="50"/>
       <c r="P7" s="44" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q7" s="51"/>
+        <v>62</v>
+      </c>
+      <c r="Q7" s="51" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="8" spans="1:18" ht="80" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
@@ -1327,25 +1334,25 @@
       <c r="A10" s="3">
         <v>46174</v>
       </c>
-      <c r="B10" s="82" t="s">
+      <c r="B10" s="77" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="80"/>
+      <c r="C10" s="78"/>
       <c r="D10" s="65"/>
-      <c r="E10" s="80" t="s">
+      <c r="E10" s="78" t="s">
         <v>23</v>
       </c>
-      <c r="F10" s="81"/>
+      <c r="F10" s="89"/>
       <c r="G10" s="68"/>
-      <c r="H10" s="83" t="s">
+      <c r="H10" s="90" t="s">
         <v>23</v>
       </c>
-      <c r="I10" s="84"/>
+      <c r="I10" s="91"/>
       <c r="J10" s="56"/>
-      <c r="K10" s="84" t="s">
+      <c r="K10" s="91" t="s">
         <v>23</v>
       </c>
-      <c r="L10" s="85"/>
+      <c r="L10" s="92"/>
       <c r="M10" s="57"/>
       <c r="N10" s="42" t="s">
         <v>27</v>
@@ -1360,25 +1367,25 @@
       <c r="A11" s="3">
         <v>46539</v>
       </c>
-      <c r="B11" s="82" t="s">
+      <c r="B11" s="77" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="80"/>
+      <c r="C11" s="78"/>
       <c r="D11" s="65"/>
-      <c r="E11" s="80" t="s">
+      <c r="E11" s="78" t="s">
         <v>29</v>
       </c>
-      <c r="F11" s="81"/>
+      <c r="F11" s="89"/>
       <c r="G11" s="68"/>
-      <c r="H11" s="83" t="s">
+      <c r="H11" s="90" t="s">
         <v>29</v>
       </c>
-      <c r="I11" s="84"/>
+      <c r="I11" s="91"/>
       <c r="J11" s="56"/>
-      <c r="K11" s="84" t="s">
+      <c r="K11" s="91" t="s">
         <v>29</v>
       </c>
-      <c r="L11" s="85"/>
+      <c r="L11" s="92"/>
       <c r="M11" s="57"/>
       <c r="N11" s="42" t="s">
         <v>28</v>
@@ -1390,45 +1397,45 @@
       <c r="Q11" s="51"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B12" s="77" t="s">
+      <c r="B12" s="86" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="78"/>
-      <c r="D12" s="78"/>
-      <c r="E12" s="78"/>
-      <c r="F12" s="78"/>
-      <c r="G12" s="78"/>
-      <c r="H12" s="78"/>
-      <c r="I12" s="78"/>
-      <c r="J12" s="78"/>
-      <c r="K12" s="78"/>
-      <c r="L12" s="78"/>
-      <c r="M12" s="78"/>
-      <c r="N12" s="78"/>
-      <c r="O12" s="78"/>
-      <c r="P12" s="78"/>
-      <c r="Q12" s="78"/>
+      <c r="C12" s="87"/>
+      <c r="D12" s="87"/>
+      <c r="E12" s="87"/>
+      <c r="F12" s="87"/>
+      <c r="G12" s="87"/>
+      <c r="H12" s="87"/>
+      <c r="I12" s="87"/>
+      <c r="J12" s="87"/>
+      <c r="K12" s="87"/>
+      <c r="L12" s="87"/>
+      <c r="M12" s="87"/>
+      <c r="N12" s="87"/>
+      <c r="O12" s="87"/>
+      <c r="P12" s="87"/>
+      <c r="Q12" s="87"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B13" s="87" t="s">
+      <c r="B13" s="71" t="s">
         <v>2</v>
       </c>
-      <c r="C13" s="88"/>
+      <c r="C13" s="72"/>
       <c r="D13" s="63"/>
-      <c r="E13" s="89" t="s">
+      <c r="E13" s="73" t="s">
         <v>3</v>
       </c>
-      <c r="F13" s="88"/>
+      <c r="F13" s="72"/>
       <c r="G13" s="63"/>
-      <c r="H13" s="92" t="s">
+      <c r="H13" s="76" t="s">
         <v>2</v>
       </c>
-      <c r="I13" s="90"/>
-      <c r="J13" s="91"/>
-      <c r="K13" s="90" t="s">
+      <c r="I13" s="74"/>
+      <c r="J13" s="75"/>
+      <c r="K13" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="L13" s="90"/>
+      <c r="L13" s="74"/>
       <c r="M13" s="10"/>
       <c r="N13" s="39" t="s">
         <v>39</v>
@@ -1555,9 +1562,9 @@
       <c r="F17" s="28"/>
       <c r="G17" s="66"/>
       <c r="L17" s="40"/>
-      <c r="N17" s="86"/>
-      <c r="O17" s="86"/>
-      <c r="P17" s="86"/>
+      <c r="N17" s="70"/>
+      <c r="O17" s="70"/>
+      <c r="P17" s="70"/>
       <c r="Q17" s="31"/>
     </row>
     <row r="18" spans="1:17" s="24" customFormat="1" x14ac:dyDescent="0.2">
@@ -3182,15 +3189,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="N17:P17"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="H13:J13"/>
-    <mergeCell ref="K13:L13"/>
-    <mergeCell ref="B10:C10"/>
     <mergeCell ref="H1:M1"/>
     <mergeCell ref="B1:G1"/>
     <mergeCell ref="B2:Q2"/>
@@ -3203,6 +3201,15 @@
     <mergeCell ref="K10:L10"/>
     <mergeCell ref="H11:I11"/>
     <mergeCell ref="K11:L11"/>
+    <mergeCell ref="N17:P17"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="H13:J13"/>
+    <mergeCell ref="K13:L13"/>
+    <mergeCell ref="B10:C10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update task status of 26 June
</commit_message>
<xml_diff>
--- a/PRD/Concrete timeline_15.06.18.xlsx
+++ b/PRD/Concrete timeline_15.06.18.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="63">
   <si>
     <t>Stella</t>
   </si>
@@ -584,6 +584,33 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="17" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -614,15 +641,9 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="17" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="17" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="17" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="17" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -631,27 +652,6 @@
     </xf>
     <xf numFmtId="17" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -936,7 +936,7 @@
   <dimension ref="A1:R197"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" zoomScale="75" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="S7" sqref="S7"/>
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -961,22 +961,22 @@
   <sheetData>
     <row r="1" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2"/>
-      <c r="B1" s="72" t="s">
+      <c r="B1" s="81" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="72"/>
-      <c r="D1" s="72"/>
-      <c r="E1" s="72"/>
-      <c r="F1" s="72"/>
-      <c r="G1" s="73"/>
-      <c r="H1" s="70" t="s">
+      <c r="C1" s="81"/>
+      <c r="D1" s="81"/>
+      <c r="E1" s="81"/>
+      <c r="F1" s="81"/>
+      <c r="G1" s="82"/>
+      <c r="H1" s="79" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="71"/>
-      <c r="J1" s="71"/>
-      <c r="K1" s="71"/>
-      <c r="L1" s="71"/>
-      <c r="M1" s="71"/>
+      <c r="I1" s="80"/>
+      <c r="J1" s="80"/>
+      <c r="K1" s="80"/>
+      <c r="L1" s="80"/>
+      <c r="M1" s="80"/>
       <c r="N1" s="38" t="s">
         <v>10</v>
       </c>
@@ -988,51 +988,51 @@
     </row>
     <row r="2" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
-      <c r="B2" s="74" t="s">
+      <c r="B2" s="83" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="75"/>
-      <c r="D2" s="75"/>
-      <c r="E2" s="75"/>
-      <c r="F2" s="75"/>
-      <c r="G2" s="75"/>
-      <c r="H2" s="75"/>
-      <c r="I2" s="75"/>
-      <c r="J2" s="75"/>
-      <c r="K2" s="75"/>
-      <c r="L2" s="75"/>
-      <c r="M2" s="75"/>
-      <c r="N2" s="75"/>
-      <c r="O2" s="75"/>
-      <c r="P2" s="75"/>
-      <c r="Q2" s="76"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="84"/>
+      <c r="G2" s="84"/>
+      <c r="H2" s="84"/>
+      <c r="I2" s="84"/>
+      <c r="J2" s="84"/>
+      <c r="K2" s="84"/>
+      <c r="L2" s="84"/>
+      <c r="M2" s="84"/>
+      <c r="N2" s="84"/>
+      <c r="O2" s="84"/>
+      <c r="P2" s="84"/>
+      <c r="Q2" s="85"/>
     </row>
     <row r="3" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="87" t="s">
+      <c r="B3" s="71" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="88"/>
+      <c r="C3" s="72"/>
       <c r="D3" s="62" t="s">
         <v>38</v>
       </c>
-      <c r="E3" s="89" t="s">
+      <c r="E3" s="73" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="88"/>
+      <c r="F3" s="72"/>
       <c r="G3" s="63" t="s">
         <v>38</v>
       </c>
-      <c r="H3" s="79" t="s">
+      <c r="H3" s="88" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="79"/>
+      <c r="I3" s="88"/>
       <c r="J3" s="52" t="s">
         <v>38</v>
       </c>
-      <c r="K3" s="90" t="s">
+      <c r="K3" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="L3" s="91"/>
+      <c r="L3" s="75"/>
       <c r="M3" s="9" t="s">
         <v>38</v>
       </c>
@@ -1180,7 +1180,9 @@
       <c r="I6" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="J6" s="53"/>
+      <c r="J6" s="53" t="s">
+        <v>40</v>
+      </c>
       <c r="K6" s="30" t="s">
         <v>37</v>
       </c>
@@ -1220,7 +1222,9 @@
       <c r="F7" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="G7" s="64"/>
+      <c r="G7" s="64" t="s">
+        <v>40</v>
+      </c>
       <c r="H7" s="20" t="s">
         <v>59</v>
       </c>
@@ -1234,7 +1238,9 @@
       <c r="L7" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="M7" s="55"/>
+      <c r="M7" s="55" t="s">
+        <v>40</v>
+      </c>
       <c r="N7" s="42" t="s">
         <v>26</v>
       </c>
@@ -1279,7 +1285,9 @@
       <c r="L8" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="M8" s="55"/>
+      <c r="M8" s="55" t="s">
+        <v>40</v>
+      </c>
       <c r="N8" s="42" t="s">
         <v>25</v>
       </c>
@@ -1342,25 +1350,25 @@
       <c r="A10" s="3">
         <v>46174</v>
       </c>
-      <c r="B10" s="82" t="s">
+      <c r="B10" s="77" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="80"/>
+      <c r="C10" s="78"/>
       <c r="D10" s="65"/>
-      <c r="E10" s="80" t="s">
+      <c r="E10" s="78" t="s">
         <v>23</v>
       </c>
-      <c r="F10" s="81"/>
+      <c r="F10" s="89"/>
       <c r="G10" s="68"/>
-      <c r="H10" s="83" t="s">
+      <c r="H10" s="90" t="s">
         <v>23</v>
       </c>
-      <c r="I10" s="84"/>
+      <c r="I10" s="91"/>
       <c r="J10" s="56"/>
-      <c r="K10" s="84" t="s">
+      <c r="K10" s="91" t="s">
         <v>23</v>
       </c>
-      <c r="L10" s="85"/>
+      <c r="L10" s="92"/>
       <c r="M10" s="57"/>
       <c r="N10" s="42" t="s">
         <v>27</v>
@@ -1375,25 +1383,25 @@
       <c r="A11" s="3">
         <v>46539</v>
       </c>
-      <c r="B11" s="82" t="s">
+      <c r="B11" s="77" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="80"/>
+      <c r="C11" s="78"/>
       <c r="D11" s="65"/>
-      <c r="E11" s="80" t="s">
+      <c r="E11" s="78" t="s">
         <v>29</v>
       </c>
-      <c r="F11" s="81"/>
+      <c r="F11" s="89"/>
       <c r="G11" s="68"/>
-      <c r="H11" s="83" t="s">
+      <c r="H11" s="90" t="s">
         <v>29</v>
       </c>
-      <c r="I11" s="84"/>
+      <c r="I11" s="91"/>
       <c r="J11" s="56"/>
-      <c r="K11" s="84" t="s">
+      <c r="K11" s="91" t="s">
         <v>29</v>
       </c>
-      <c r="L11" s="85"/>
+      <c r="L11" s="92"/>
       <c r="M11" s="57"/>
       <c r="N11" s="42" t="s">
         <v>28</v>
@@ -1405,45 +1413,45 @@
       <c r="Q11" s="51"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B12" s="77" t="s">
+      <c r="B12" s="86" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="78"/>
-      <c r="D12" s="78"/>
-      <c r="E12" s="78"/>
-      <c r="F12" s="78"/>
-      <c r="G12" s="78"/>
-      <c r="H12" s="78"/>
-      <c r="I12" s="78"/>
-      <c r="J12" s="78"/>
-      <c r="K12" s="78"/>
-      <c r="L12" s="78"/>
-      <c r="M12" s="78"/>
-      <c r="N12" s="78"/>
-      <c r="O12" s="78"/>
-      <c r="P12" s="78"/>
-      <c r="Q12" s="78"/>
+      <c r="C12" s="87"/>
+      <c r="D12" s="87"/>
+      <c r="E12" s="87"/>
+      <c r="F12" s="87"/>
+      <c r="G12" s="87"/>
+      <c r="H12" s="87"/>
+      <c r="I12" s="87"/>
+      <c r="J12" s="87"/>
+      <c r="K12" s="87"/>
+      <c r="L12" s="87"/>
+      <c r="M12" s="87"/>
+      <c r="N12" s="87"/>
+      <c r="O12" s="87"/>
+      <c r="P12" s="87"/>
+      <c r="Q12" s="87"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B13" s="87" t="s">
+      <c r="B13" s="71" t="s">
         <v>2</v>
       </c>
-      <c r="C13" s="88"/>
+      <c r="C13" s="72"/>
       <c r="D13" s="63"/>
-      <c r="E13" s="89" t="s">
+      <c r="E13" s="73" t="s">
         <v>3</v>
       </c>
-      <c r="F13" s="88"/>
+      <c r="F13" s="72"/>
       <c r="G13" s="63"/>
-      <c r="H13" s="92" t="s">
+      <c r="H13" s="76" t="s">
         <v>2</v>
       </c>
-      <c r="I13" s="90"/>
-      <c r="J13" s="91"/>
-      <c r="K13" s="90" t="s">
+      <c r="I13" s="74"/>
+      <c r="J13" s="75"/>
+      <c r="K13" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="L13" s="90"/>
+      <c r="L13" s="74"/>
       <c r="M13" s="10"/>
       <c r="N13" s="39" t="s">
         <v>39</v>
@@ -1570,9 +1578,9 @@
       <c r="F17" s="28"/>
       <c r="G17" s="66"/>
       <c r="L17" s="40"/>
-      <c r="N17" s="86"/>
-      <c r="O17" s="86"/>
-      <c r="P17" s="86"/>
+      <c r="N17" s="70"/>
+      <c r="O17" s="70"/>
+      <c r="P17" s="70"/>
       <c r="Q17" s="31"/>
     </row>
     <row r="18" spans="1:17" s="24" customFormat="1" x14ac:dyDescent="0.2">
@@ -3197,15 +3205,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="N17:P17"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="H13:J13"/>
-    <mergeCell ref="K13:L13"/>
-    <mergeCell ref="B10:C10"/>
     <mergeCell ref="H1:M1"/>
     <mergeCell ref="B1:G1"/>
     <mergeCell ref="B2:Q2"/>
@@ -3218,6 +3217,15 @@
     <mergeCell ref="K10:L10"/>
     <mergeCell ref="H11:I11"/>
     <mergeCell ref="K11:L11"/>
+    <mergeCell ref="N17:P17"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="H13:J13"/>
+    <mergeCell ref="K13:L13"/>
+    <mergeCell ref="B10:C10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update task status for wanlu and stella
</commit_message>
<xml_diff>
--- a/PRD/Concrete timeline_15.06.18.xlsx
+++ b/PRD/Concrete timeline_15.06.18.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="64">
   <si>
     <t>Stella</t>
   </si>
@@ -220,6 +220,11 @@
     <t>Critical feedback on previous day's work: 1. Please revise scale according to this example  https://wkwsci.co1.qualtrics.com/jfe/form/SV_eP3DmZu9T34ChqB
 2. Change visual advisor to “your personal financial advisor”
 3. Stage 0: both of Study and Conditions need to be highlighted</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Work on unfinished parts of previous days
+1. Prepare for the online version of the experiment (using automatic randomization process)
+2. Create a separte link for the online version </t>
   </si>
 </sst>
 </file>
@@ -584,6 +589,54 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="17" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="17" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="17" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="17" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="17" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -604,54 +657,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="17" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="17" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="17" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="17" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -935,8 +940,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R197"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="75" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="75" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10:L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -961,22 +966,22 @@
   <sheetData>
     <row r="1" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2"/>
-      <c r="B1" s="81" t="s">
+      <c r="B1" s="72" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="81"/>
-      <c r="D1" s="81"/>
-      <c r="E1" s="81"/>
-      <c r="F1" s="81"/>
-      <c r="G1" s="82"/>
-      <c r="H1" s="79" t="s">
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
+      <c r="E1" s="72"/>
+      <c r="F1" s="72"/>
+      <c r="G1" s="73"/>
+      <c r="H1" s="70" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="80"/>
-      <c r="J1" s="80"/>
-      <c r="K1" s="80"/>
-      <c r="L1" s="80"/>
-      <c r="M1" s="80"/>
+      <c r="I1" s="71"/>
+      <c r="J1" s="71"/>
+      <c r="K1" s="71"/>
+      <c r="L1" s="71"/>
+      <c r="M1" s="71"/>
       <c r="N1" s="38" t="s">
         <v>10</v>
       </c>
@@ -988,51 +993,51 @@
     </row>
     <row r="2" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
-      <c r="B2" s="83" t="s">
+      <c r="B2" s="74" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="84"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
-      <c r="F2" s="84"/>
-      <c r="G2" s="84"/>
-      <c r="H2" s="84"/>
-      <c r="I2" s="84"/>
-      <c r="J2" s="84"/>
-      <c r="K2" s="84"/>
-      <c r="L2" s="84"/>
-      <c r="M2" s="84"/>
-      <c r="N2" s="84"/>
-      <c r="O2" s="84"/>
-      <c r="P2" s="84"/>
-      <c r="Q2" s="85"/>
+      <c r="C2" s="75"/>
+      <c r="D2" s="75"/>
+      <c r="E2" s="75"/>
+      <c r="F2" s="75"/>
+      <c r="G2" s="75"/>
+      <c r="H2" s="75"/>
+      <c r="I2" s="75"/>
+      <c r="J2" s="75"/>
+      <c r="K2" s="75"/>
+      <c r="L2" s="75"/>
+      <c r="M2" s="75"/>
+      <c r="N2" s="75"/>
+      <c r="O2" s="75"/>
+      <c r="P2" s="75"/>
+      <c r="Q2" s="76"/>
     </row>
     <row r="3" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="71" t="s">
+      <c r="B3" s="87" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="72"/>
+      <c r="C3" s="88"/>
       <c r="D3" s="62" t="s">
         <v>38</v>
       </c>
-      <c r="E3" s="73" t="s">
+      <c r="E3" s="89" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="72"/>
+      <c r="F3" s="88"/>
       <c r="G3" s="63" t="s">
         <v>38</v>
       </c>
-      <c r="H3" s="88" t="s">
+      <c r="H3" s="79" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="88"/>
+      <c r="I3" s="79"/>
       <c r="J3" s="52" t="s">
         <v>38</v>
       </c>
-      <c r="K3" s="74" t="s">
+      <c r="K3" s="90" t="s">
         <v>3</v>
       </c>
-      <c r="L3" s="75"/>
+      <c r="L3" s="91"/>
       <c r="M3" s="9" t="s">
         <v>38</v>
       </c>
@@ -1346,29 +1351,29 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18" ht="67" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>46174</v>
       </c>
-      <c r="B10" s="77" t="s">
+      <c r="B10" s="82" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="78"/>
+      <c r="C10" s="80"/>
       <c r="D10" s="65"/>
-      <c r="E10" s="78" t="s">
+      <c r="E10" s="80" t="s">
         <v>23</v>
       </c>
-      <c r="F10" s="89"/>
+      <c r="F10" s="81"/>
       <c r="G10" s="68"/>
-      <c r="H10" s="90" t="s">
+      <c r="H10" s="83" t="s">
         <v>23</v>
       </c>
-      <c r="I10" s="91"/>
+      <c r="I10" s="84"/>
       <c r="J10" s="56"/>
-      <c r="K10" s="91" t="s">
-        <v>23</v>
-      </c>
-      <c r="L10" s="92"/>
+      <c r="K10" s="84" t="s">
+        <v>63</v>
+      </c>
+      <c r="L10" s="85"/>
       <c r="M10" s="57"/>
       <c r="N10" s="42" t="s">
         <v>27</v>
@@ -1383,25 +1388,25 @@
       <c r="A11" s="3">
         <v>46539</v>
       </c>
-      <c r="B11" s="77" t="s">
+      <c r="B11" s="82" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="78"/>
+      <c r="C11" s="80"/>
       <c r="D11" s="65"/>
-      <c r="E11" s="78" t="s">
+      <c r="E11" s="80" t="s">
         <v>29</v>
       </c>
-      <c r="F11" s="89"/>
+      <c r="F11" s="81"/>
       <c r="G11" s="68"/>
-      <c r="H11" s="90" t="s">
+      <c r="H11" s="83" t="s">
         <v>29</v>
       </c>
-      <c r="I11" s="91"/>
+      <c r="I11" s="84"/>
       <c r="J11" s="56"/>
-      <c r="K11" s="91" t="s">
+      <c r="K11" s="84" t="s">
         <v>29</v>
       </c>
-      <c r="L11" s="92"/>
+      <c r="L11" s="85"/>
       <c r="M11" s="57"/>
       <c r="N11" s="42" t="s">
         <v>28</v>
@@ -1413,45 +1418,45 @@
       <c r="Q11" s="51"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B12" s="86" t="s">
+      <c r="B12" s="77" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="87"/>
-      <c r="D12" s="87"/>
-      <c r="E12" s="87"/>
-      <c r="F12" s="87"/>
-      <c r="G12" s="87"/>
-      <c r="H12" s="87"/>
-      <c r="I12" s="87"/>
-      <c r="J12" s="87"/>
-      <c r="K12" s="87"/>
-      <c r="L12" s="87"/>
-      <c r="M12" s="87"/>
-      <c r="N12" s="87"/>
-      <c r="O12" s="87"/>
-      <c r="P12" s="87"/>
-      <c r="Q12" s="87"/>
+      <c r="C12" s="78"/>
+      <c r="D12" s="78"/>
+      <c r="E12" s="78"/>
+      <c r="F12" s="78"/>
+      <c r="G12" s="78"/>
+      <c r="H12" s="78"/>
+      <c r="I12" s="78"/>
+      <c r="J12" s="78"/>
+      <c r="K12" s="78"/>
+      <c r="L12" s="78"/>
+      <c r="M12" s="78"/>
+      <c r="N12" s="78"/>
+      <c r="O12" s="78"/>
+      <c r="P12" s="78"/>
+      <c r="Q12" s="78"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B13" s="71" t="s">
+      <c r="B13" s="87" t="s">
         <v>2</v>
       </c>
-      <c r="C13" s="72"/>
+      <c r="C13" s="88"/>
       <c r="D13" s="63"/>
-      <c r="E13" s="73" t="s">
+      <c r="E13" s="89" t="s">
         <v>3</v>
       </c>
-      <c r="F13" s="72"/>
+      <c r="F13" s="88"/>
       <c r="G13" s="63"/>
-      <c r="H13" s="76" t="s">
+      <c r="H13" s="92" t="s">
         <v>2</v>
       </c>
-      <c r="I13" s="74"/>
-      <c r="J13" s="75"/>
-      <c r="K13" s="74" t="s">
+      <c r="I13" s="90"/>
+      <c r="J13" s="91"/>
+      <c r="K13" s="90" t="s">
         <v>3</v>
       </c>
-      <c r="L13" s="74"/>
+      <c r="L13" s="90"/>
       <c r="M13" s="10"/>
       <c r="N13" s="39" t="s">
         <v>39</v>
@@ -1578,9 +1583,9 @@
       <c r="F17" s="28"/>
       <c r="G17" s="66"/>
       <c r="L17" s="40"/>
-      <c r="N17" s="70"/>
-      <c r="O17" s="70"/>
-      <c r="P17" s="70"/>
+      <c r="N17" s="86"/>
+      <c r="O17" s="86"/>
+      <c r="P17" s="86"/>
       <c r="Q17" s="31"/>
     </row>
     <row r="18" spans="1:17" s="24" customFormat="1" x14ac:dyDescent="0.2">
@@ -3205,6 +3210,15 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="N17:P17"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="H13:J13"/>
+    <mergeCell ref="K13:L13"/>
+    <mergeCell ref="B10:C10"/>
     <mergeCell ref="H1:M1"/>
     <mergeCell ref="B1:G1"/>
     <mergeCell ref="B2:Q2"/>
@@ -3217,15 +3231,6 @@
     <mergeCell ref="K10:L10"/>
     <mergeCell ref="H11:I11"/>
     <mergeCell ref="K11:L11"/>
-    <mergeCell ref="N17:P17"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="H13:J13"/>
-    <mergeCell ref="K13:L13"/>
-    <mergeCell ref="B10:C10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>